<commit_message>
upates to indexing and packaging code
</commit_message>
<xml_diff>
--- a/CSDCODirWalkTests/godirwalk/Book1.xlsx
+++ b/CSDCODirWalkTests/godirwalk/Book1.xlsx
@@ -327,31 +327,31 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>/z2c/file2c1</v>
+        <v>/dir1a/z1a2</v>
       </c>
       <c r="B1" t="str"/>
       <c r="C1" t="str">
         <v>notvalid</v>
       </c>
       <c r="D1" t="str">
-        <v>dir2</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>/dir1a/z1a2</v>
+        <v>/z2c/file2c1</v>
       </c>
       <c r="B2" t="str"/>
       <c r="C2" t="str">
         <v>notvalid</v>
       </c>
       <c r="D2" t="str">
-        <v>dir1</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>/dir1a/file1a1</v>
+        <v>/dir1a/z1a2</v>
       </c>
       <c r="B3" t="str"/>
       <c r="C3" t="str">
@@ -363,19 +363,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>/a2/a2b.txt</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B4" t="str"/>
       <c r="C4" t="str">
         <v>notvalid</v>
       </c>
       <c r="D4" t="str">
-        <v>dir5</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>/dir1a/skip</v>
+        <v>/dir1a/z1a2</v>
       </c>
       <c r="B5" t="str"/>
       <c r="C5" t="str">
@@ -387,62 +387,62 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/a2/a2b.txt</v>
       </c>
       <c r="B6" t="str"/>
       <c r="C6" t="str">
         <v>notvalid</v>
       </c>
       <c r="D6" t="str">
-        <v>dir4</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>/skip/file2b1</v>
+        <v>/dir1a/file1a1</v>
       </c>
       <c r="B7" t="str"/>
       <c r="C7" t="str">
         <v>notvalid</v>
       </c>
       <c r="D7" t="str">
-        <v>dir2</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>/skip/file2b1</v>
+        <v>/a2/a2a/a2a1.txt</v>
       </c>
       <c r="B8" t="str"/>
       <c r="C8" t="str">
         <v>notvalid</v>
       </c>
       <c r="D8" t="str">
-        <v>dir2</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/dir1a/z1a2</v>
       </c>
       <c r="B9" t="str"/>
       <c r="C9" t="str">
         <v>notvalid</v>
       </c>
       <c r="D9" t="str">
-        <v>dir3</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>/z2c/file2c1</v>
+        <v>/dir1a/skip</v>
       </c>
       <c r="B10" t="str"/>
       <c r="C10" t="str">
         <v>notvalid</v>
       </c>
       <c r="D10" t="str">
-        <v>dir2</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="11">
@@ -459,170 +459,170 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>/dir1a/skip</v>
+        <v>/a2/a2b.txt</v>
       </c>
       <c r="B12" t="str"/>
       <c r="C12" t="str">
         <v>notvalid</v>
       </c>
       <c r="D12" t="str">
-        <v>dir1</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>/a2/a2a/a2a1.txt</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B13" t="str"/>
       <c r="C13" t="str">
         <v>notvalid</v>
       </c>
       <c r="D13" t="str">
-        <v>dir5</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>/dir1a/z1a2</v>
+        <v>/a2/a2b.txt</v>
       </c>
       <c r="B14" t="str"/>
       <c r="C14" t="str">
         <v>notvalid</v>
       </c>
       <c r="D14" t="str">
-        <v>dir1</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>/skip/file2b1</v>
+        <v>/dir1a/skip</v>
       </c>
       <c r="B15" t="str"/>
       <c r="C15" t="str">
         <v>notvalid</v>
       </c>
       <c r="D15" t="str">
-        <v>dir2</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>/a2/a2a/a2a1.txt</v>
+        <v>/zzz/aaa.txt</v>
       </c>
       <c r="B16" t="str"/>
       <c r="C16" t="str">
         <v>notvalid</v>
       </c>
       <c r="D16" t="str">
-        <v>dir5</v>
+        <v>dir3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>/dir1a/skip</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B17" t="str"/>
       <c r="C17" t="str">
         <v>notvalid</v>
       </c>
       <c r="D17" t="str">
-        <v>dir1</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>/a2/a2b.txt</v>
+        <v>/zzz/aaa.txt</v>
       </c>
       <c r="B18" t="str"/>
       <c r="C18" t="str">
         <v>notvalid</v>
       </c>
       <c r="D18" t="str">
-        <v>dir5</v>
+        <v>dir4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>/z2c/file2c1</v>
+        <v>/a2/a2a/a2a1.txt</v>
       </c>
       <c r="B19" t="str"/>
       <c r="C19" t="str">
         <v>notvalid</v>
       </c>
       <c r="D19" t="str">
-        <v>dir2</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/dir1a/skip</v>
       </c>
       <c r="B20" t="str"/>
       <c r="C20" t="str">
         <v>notvalid</v>
       </c>
       <c r="D20" t="str">
-        <v>dir3</v>
+        <v>dir1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>/a2/a2a/a2a1.txt</v>
+        <v>/zzz/aaa.txt</v>
       </c>
       <c r="B21" t="str"/>
       <c r="C21" t="str">
         <v>notvalid</v>
       </c>
       <c r="D21" t="str">
-        <v>dir5</v>
+        <v>dir4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>/dir1a/file1a1</v>
+        <v>/a2/a2b.txt</v>
       </c>
       <c r="B22" t="str"/>
       <c r="C22" t="str">
         <v>notvalid</v>
       </c>
       <c r="D22" t="str">
-        <v>dir1</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B23" t="str"/>
       <c r="C23" t="str">
         <v>notvalid</v>
       </c>
       <c r="D23" t="str">
-        <v>dir3</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/a2/a2b.txt</v>
       </c>
       <c r="B24" t="str"/>
       <c r="C24" t="str">
         <v>notvalid</v>
       </c>
       <c r="D24" t="str">
-        <v>dir4</v>
+        <v>dir5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>/zzz/aaa.txt</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B25" t="str"/>
       <c r="C25" t="str">
         <v>notvalid</v>
       </c>
       <c r="D25" t="str">
-        <v>dir4</v>
+        <v>dir2</v>
       </c>
     </row>
     <row r="26">
@@ -639,13 +639,985 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>/dir1a/z1a2</v>
+        <v>/skip/file2b1</v>
       </c>
       <c r="B27" t="str"/>
       <c r="C27" t="str">
         <v>notvalid</v>
       </c>
       <c r="D27" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B28" t="str"/>
+      <c r="C28" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D28" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B29" t="str"/>
+      <c r="C29" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D29" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B30" t="str"/>
+      <c r="C30" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D30" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B31" t="str"/>
+      <c r="C31" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D31" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B32" t="str"/>
+      <c r="C32" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D32" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B33" t="str"/>
+      <c r="C33" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D33" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B34" t="str"/>
+      <c r="C34" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D34" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B35" t="str"/>
+      <c r="C35" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D35" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B36" t="str"/>
+      <c r="C36" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D36" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B37" t="str"/>
+      <c r="C37" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D37" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B38" t="str"/>
+      <c r="C38" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D38" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B39" t="str"/>
+      <c r="C39" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D39" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B40" t="str"/>
+      <c r="C40" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D40" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B41" t="str"/>
+      <c r="C41" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D41" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B42" t="str"/>
+      <c r="C42" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D42" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B43" t="str"/>
+      <c r="C43" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D43" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B44" t="str"/>
+      <c r="C44" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D44" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B45" t="str"/>
+      <c r="C45" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D45" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B46" t="str"/>
+      <c r="C46" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D46" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B47" t="str"/>
+      <c r="C47" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D47" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B48" t="str"/>
+      <c r="C48" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D48" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B49" t="str"/>
+      <c r="C49" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D49" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B50" t="str"/>
+      <c r="C50" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D50" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B51" t="str"/>
+      <c r="C51" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D51" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B52" t="str"/>
+      <c r="C52" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D52" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B53" t="str"/>
+      <c r="C53" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D53" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B54" t="str"/>
+      <c r="C54" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D54" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B55" t="str"/>
+      <c r="C55" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D55" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B56" t="str"/>
+      <c r="C56" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D56" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B57" t="str"/>
+      <c r="C57" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D57" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B58" t="str"/>
+      <c r="C58" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D58" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B59" t="str"/>
+      <c r="C59" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D59" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B60" t="str"/>
+      <c r="C60" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D60" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B61" t="str"/>
+      <c r="C61" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D61" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B62" t="str"/>
+      <c r="C62" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D62" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B63" t="str"/>
+      <c r="C63" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D63" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B64" t="str"/>
+      <c r="C64" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D64" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B65" t="str"/>
+      <c r="C65" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D65" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B66" t="str"/>
+      <c r="C66" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D66" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B67" t="str"/>
+      <c r="C67" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D67" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B68" t="str"/>
+      <c r="C68" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D68" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B69" t="str"/>
+      <c r="C69" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D69" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B70" t="str"/>
+      <c r="C70" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D70" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B71" t="str"/>
+      <c r="C71" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D71" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B72" t="str"/>
+      <c r="C72" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D72" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B73" t="str"/>
+      <c r="C73" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D73" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B74" t="str"/>
+      <c r="C74" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D74" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B75" t="str"/>
+      <c r="C75" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D75" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B76" t="str"/>
+      <c r="C76" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D76" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B77" t="str"/>
+      <c r="C77" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D77" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B78" t="str"/>
+      <c r="C78" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D78" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B79" t="str"/>
+      <c r="C79" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D79" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B80" t="str"/>
+      <c r="C80" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D80" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B81" t="str"/>
+      <c r="C81" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D81" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B82" t="str"/>
+      <c r="C82" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D82" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B83" t="str"/>
+      <c r="C83" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D83" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B84" t="str"/>
+      <c r="C84" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D84" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>/skip/file2b1</v>
+      </c>
+      <c r="B85" t="str"/>
+      <c r="C85" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D85" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B86" t="str"/>
+      <c r="C86" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D86" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B87" t="str"/>
+      <c r="C87" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D87" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B88" t="str"/>
+      <c r="C88" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D88" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B89" t="str"/>
+      <c r="C89" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D89" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B90" t="str"/>
+      <c r="C90" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D90" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>/a2/a2a/a2a1.txt</v>
+      </c>
+      <c r="B91" t="str"/>
+      <c r="C91" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D91" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B92" t="str"/>
+      <c r="C92" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D92" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B93" t="str"/>
+      <c r="C93" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D93" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B94" t="str"/>
+      <c r="C94" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D94" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B95" t="str"/>
+      <c r="C95" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D95" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B96" t="str"/>
+      <c r="C96" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D96" t="str">
+        <v>dir3</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B97" t="str"/>
+      <c r="C97" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D97" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B98" t="str"/>
+      <c r="C98" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D98" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B99" t="str"/>
+      <c r="C99" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D99" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B100" t="str"/>
+      <c r="C100" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D100" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>/dir1a/skip</v>
+      </c>
+      <c r="B101" t="str"/>
+      <c r="C101" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D101" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B102" t="str"/>
+      <c r="C102" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D102" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B103" t="str"/>
+      <c r="C103" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D103" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>/zzz/aaa.txt</v>
+      </c>
+      <c r="B104" t="str"/>
+      <c r="C104" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D104" t="str">
+        <v>dir4</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>/a2/a2b.txt</v>
+      </c>
+      <c r="B105" t="str"/>
+      <c r="C105" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D105" t="str">
+        <v>dir5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>/dir1a/file1a1</v>
+      </c>
+      <c r="B106" t="str"/>
+      <c r="C106" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D106" t="str">
+        <v>dir1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>/z2c/file2c1</v>
+      </c>
+      <c r="B107" t="str"/>
+      <c r="C107" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D107" t="str">
+        <v>dir2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>/dir1a/z1a2</v>
+      </c>
+      <c r="B108" t="str"/>
+      <c r="C108" t="str">
+        <v>notvalid</v>
+      </c>
+      <c r="D108" t="str">
         <v>dir1</v>
       </c>
     </row>

</xml_diff>